<commit_message>
Pass up cyclic dimensions when coarsening for 1st time, plus more tests
</commit_message>
<xml_diff>
--- a/Docs/UnitTests/MultigridLayerDemos.xlsx
+++ b/Docs/UnitTests/MultigridLayerDemos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Finer</t>
   </si>
@@ -174,8 +174,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -202,17 +226,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -220,6 +244,18 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -227,6 +263,18 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Z19"/>
+  <dimension ref="A3:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,66 +632,66 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:26" ht="20">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="11" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="J4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="S4" s="11" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="S4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5">
@@ -764,7 +812,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7">
-        <f t="shared" ref="A7:A12" si="2">A6+8</f>
+        <f>A6+8</f>
         <v>16</v>
       </c>
       <c r="B7">
@@ -826,7 +874,7 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A8:A12" si="2">A7+8</f>
         <v>24</v>
       </c>
       <c r="B8">
@@ -1104,9 +1152,9 @@
       <c r="Y12" s="9"/>
       <c r="Z12" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="20">
+    <row r="14" spans="1:26">
       <c r="A14" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -1115,8 +1163,9 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="J14" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -1124,287 +1173,510 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="2"/>
+      <c r="J15" s="1">
+        <f>A15</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="1">
+        <f>(L21+N15+L17+J15)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="1">
+        <f>E15</f>
+        <v>2</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="1">
+        <f>(P21+J15+P17+N15)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="4"/>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="1">
+        <f>(J15+L17+J19+P17)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="1">
+        <f>A15</f>
+        <v>1</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="1">
+        <f>(N15+P17+N19+L17)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="1">
+        <f>E15</f>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="3"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="2"/>
+      <c r="J19" s="1">
+        <f>A19</f>
+        <v>2</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="1">
+        <f>(L17+N19+L21+J19)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="1">
+        <f>E19</f>
+        <v>1</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="1">
+        <f>(P17+J19+P21+N19)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="J21" s="1">
+        <f>(J19+L21+J15+P21)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="1">
+        <f>A19</f>
+        <v>2</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="1">
+        <f>(N19+P21+N15+L21)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="1">
+        <f>E19</f>
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" s="3"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="26" spans="1:26" ht="20">
+      <c r="A26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10"/>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="J15" s="11" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="J27" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="S15" s="11" t="s">
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="S27" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="A16">
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28">
         <v>0</v>
       </c>
-      <c r="B16">
-        <f t="shared" ref="B16:B19" si="3">A16+1</f>
+      <c r="B28">
+        <f t="shared" ref="B28:B31" si="3">A28+1</f>
         <v>1</v>
       </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C19" si="4">B16+1</f>
+      <c r="C28">
+        <f t="shared" ref="C28:C31" si="4">B28+1</f>
         <v>2</v>
       </c>
-      <c r="D16">
-        <f t="shared" ref="D16:D19" si="5">C16+1</f>
+      <c r="D28">
+        <f t="shared" ref="D28:D31" si="5">C28+1</f>
         <v>3</v>
       </c>
-      <c r="E16">
-        <f t="shared" ref="E16:E19" si="6">D16+1</f>
+      <c r="E28">
+        <f t="shared" ref="E28:E31" si="6">D28+1</f>
         <v>4</v>
       </c>
-      <c r="F16">
-        <f t="shared" ref="F16:F19" si="7">E16+1</f>
+      <c r="F28">
+        <f t="shared" ref="F28:F31" si="7">E28+1</f>
         <v>5</v>
       </c>
-      <c r="G16">
-        <f t="shared" ref="G16:G19" si="8">F16+1</f>
+      <c r="G28">
+        <f t="shared" ref="G28:G31" si="8">F28+1</f>
         <v>6</v>
       </c>
-      <c r="H16">
-        <f t="shared" ref="H16:H19" si="9">G16+1</f>
+      <c r="H28">
+        <f t="shared" ref="H28:H31" si="9">G28+1</f>
         <v>7</v>
       </c>
-      <c r="J16" s="1">
-        <f>SUM(A16:B17)*0.25</f>
+      <c r="J28" s="1">
+        <f>SUM(A28:B29)*0.25</f>
         <v>4.5</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="1">
-        <f>SUM(C16:D17)*0.25</f>
+      <c r="K28" s="2"/>
+      <c r="L28" s="1">
+        <f>SUM(C28:D29)*0.25</f>
         <v>6.5</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="1">
-        <f>SUM(E16:F17)*0.25</f>
+      <c r="M28" s="2"/>
+      <c r="N28" s="1">
+        <f>SUM(E28:F29)*0.25</f>
         <v>8.5</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="1">
-        <f>SUM(G16:H17)*0.25</f>
+      <c r="O28" s="2"/>
+      <c r="P28" s="1">
+        <f>SUM(G28:H29)*0.25</f>
         <v>10.5</v>
       </c>
-      <c r="Q16" s="2"/>
-      <c r="S16" s="1">
-        <f>SUM(J16:M19)*0.25</f>
+      <c r="Q28" s="2"/>
+      <c r="S28" s="1">
+        <f>SUM(J28:M31)*0.25</f>
         <v>13.5</v>
       </c>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="1">
-        <f>SUM(N16:Q19)*0.25</f>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="1">
+        <f>SUM(N28:Q31)*0.25</f>
         <v>17.5</v>
       </c>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="2"/>
-    </row>
-    <row r="17" spans="1:26">
-      <c r="A17">
-        <f>A16+8</f>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="2"/>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29">
+        <f>A28+8</f>
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B29">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="C17">
+      <c r="C29">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="D17">
+      <c r="D29">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="E17">
+      <c r="E29">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="F17">
+      <c r="F29">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="G17">
+      <c r="G29">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="H17">
+      <c r="H29">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="4"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="6"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="8"/>
-    </row>
-    <row r="18" spans="1:26">
-      <c r="A18">
-        <f t="shared" ref="A18:A19" si="10">A17+8</f>
+      <c r="J29" s="3"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="4"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30">
+        <f t="shared" ref="A30:A31" si="10">A29+8</f>
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B30">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C30">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="D18">
+      <c r="D30">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="E18">
+      <c r="E30">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="F18">
+      <c r="F30">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="G18">
+      <c r="G30">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="H18">
+      <c r="H30">
         <f t="shared" si="9"/>
         <v>23</v>
       </c>
-      <c r="J18" s="1">
-        <f>SUM(A18:B19)*0.25</f>
+      <c r="J30" s="1">
+        <f>SUM(A30:B31)*0.25</f>
         <v>20.5</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="1">
-        <f>SUM(C18:D19)*0.25</f>
+      <c r="K30" s="2"/>
+      <c r="L30" s="1">
+        <f>SUM(C30:D31)*0.25</f>
         <v>22.5</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="1">
-        <f>SUM(E18:F19)*0.25</f>
+      <c r="M30" s="2"/>
+      <c r="N30" s="1">
+        <f>SUM(E30:F31)*0.25</f>
         <v>24.5</v>
       </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="1">
-        <f>SUM(G18:H19)*0.25</f>
+      <c r="O30" s="2"/>
+      <c r="P30" s="1">
+        <f>SUM(G30:H31)*0.25</f>
         <v>26.5</v>
       </c>
-      <c r="Q18" s="2"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="8"/>
-    </row>
-    <row r="19" spans="1:26">
-      <c r="A19">
+      <c r="Q30" s="2"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B31">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="C19">
+      <c r="C31">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="D19">
+      <c r="D31">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="E19">
+      <c r="E31">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="F19">
+      <c r="F31">
         <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="G19">
+      <c r="G31">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H31">
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="4"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="4"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A3:Z3"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="J4:Q4"/>
     <mergeCell ref="S4:Z4"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="J15:Q15"/>
-    <mergeCell ref="S15:Z15"/>
-    <mergeCell ref="A14:Z14"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="J27:Q27"/>
+    <mergeCell ref="S27:Z27"/>
+    <mergeCell ref="A26:Z26"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="J14:Q14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>